<commit_message>
Change from Children URI to Parent IRIs column in xslx
</commit_message>
<xml_diff>
--- a/tests/data/concept-scheme-duplicates.xlsx
+++ b/tests/data/concept-scheme-duplicates.xlsx
@@ -5399,7 +5399,7 @@
       </c>
       <c r="G2" s="16" t="inlineStr">
         <is>
-          <t>Children IRIs</t>
+          <t>Parent IRIs</t>
         </is>
       </c>
       <c r="H2" s="12" t="inlineStr">
@@ -5444,11 +5444,7 @@
           <t>AltLbl for term1</t>
         </is>
       </c>
-      <c r="G3" s="24" t="inlineStr">
-        <is>
-          <t>ex:test02, ex:test03</t>
-        </is>
-      </c>
+      <c r="G3" s="24" t="n"/>
       <c r="H3" s="27" t="inlineStr">
         <is>
           <t>0000-0001-2345-6789</t>
@@ -5536,7 +5532,7 @@
       </c>
       <c r="G5" s="28" t="inlineStr">
         <is>
-          <t>ex:test04</t>
+          <t>ex:test01</t>
         </is>
       </c>
       <c r="H5" s="27" t="inlineStr">
@@ -5581,7 +5577,11 @@
           <t>AltLbl for term4</t>
         </is>
       </c>
-      <c r="G6" s="28" t="n"/>
+      <c r="G6" s="28" t="inlineStr">
+        <is>
+          <t>ex:test03</t>
+        </is>
+      </c>
       <c r="H6" s="27" t="inlineStr">
         <is>
           <t>sofia-garcia</t>

</xml_diff>